<commit_message>
layout ja käyttöliittymän suunnittelmia
</commit_message>
<xml_diff>
--- a/kirjasto-sovellus aikakirjanpito.xlsx
+++ b/kirjasto-sovellus aikakirjanpito.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Päiväys</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>Käyttöliittymän ja ulkoasun suunnittelua</t>
+  </si>
+  <si>
+    <t>Käyttöliittymän ja ulkoasun suunnittelu jatkuu, mobiilin ulkoasu valmis</t>
   </si>
 </sst>
 </file>
@@ -409,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,6 +453,17 @@
       </c>
       <c r="F2" s="3">
         <f>SUM(B2:B216)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>44015</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>